<commit_message>
work on creating link file
</commit_message>
<xml_diff>
--- a/_ETC/time-estimates/patient-counts.xlsx
+++ b/_ETC/time-estimates/patient-counts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_WORKSPACES\_ECLIPSE_WORKSPACE\workspace\GPPRL\_ETC\time-estimates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205AEC93-620B-47A3-A86E-9603B34AE9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78774336-44D1-4B73-A810-8E6DA43598CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13404" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,9 +67,6 @@
     <t># of calculations</t>
   </si>
   <si>
-    <t># sum of calculations</t>
-  </si>
-  <si>
     <t>% observed</t>
   </si>
   <si>
@@ -80,6 +77,9 @@
   </si>
   <si>
     <t>days</t>
+  </si>
+  <si>
+    <t>sum of calculations</t>
   </si>
 </sst>
 </file>
@@ -957,17 +957,18 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="17.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="9"/>
-    <col min="2" max="2" width="13.77734375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" style="9" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.88671875" style="12"/>
-    <col min="10" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="17.33203125" style="9"/>
+    <col min="2" max="2" width="13.6640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="9"/>
+    <col min="4" max="4" width="17.33203125" style="10"/>
+    <col min="5" max="5" width="20" style="10" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="9"/>
+    <col min="7" max="7" width="14" style="11" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" style="12" customWidth="1"/>
+    <col min="9" max="9" width="8.5546875" style="12" customWidth="1"/>
+    <col min="10" max="16384" width="17.33203125" style="9"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
@@ -981,19 +982,19 @@
         <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">

</xml_diff>